<commit_message>
Update ink recycling test file and test function
</commit_message>
<xml_diff>
--- a/tests/data/20250616_ink_recycling_test.xlsx
+++ b/tests/data/20250616_ink_recycling_test.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="296">
   <si>
     <t xml:space="preserve">Experiment Info</t>
   </si>
@@ -150,6 +150,21 @@
     <t xml:space="preserve">Test recycling process</t>
   </si>
   <si>
+    <t xml:space="preserve">27-05-2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DMF 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PbI2 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAI 3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Perovskite Solar Cell Fabrication Sequence</t>
   </si>
   <si>
@@ -232,9 +247,6 @@
   </si>
   <si>
     <t xml:space="preserve">Subset for variations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
   </si>
   <si>
     <t xml:space="preserve">Sample serial number</t>
@@ -1290,10 +1302,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB3"/>
+  <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T4" activeCellId="0" sqref="4:4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AB8" activeCellId="0" sqref="AB8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1535,6 +1547,180 @@
         <v>41</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1" t="str">
+        <f aca="false">CONCATENATE("HZB_",B4,"_",C4,"_",D4,"_C-",E4)</f>
+        <v>HZB_FiNa_1_1_C-2</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="N4" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="O4" s="1" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q4" s="1" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S4" s="1" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U4" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="V4" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="X4" s="1" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="Y4" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Z4" s="1" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="AA4" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1" t="str">
+        <f aca="false">CONCATENATE("HZB_",B5,"_",C5,"_",D5,"_C-",E5)</f>
+        <v>HZB_FiNa_2_2_C-3</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="1" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="N5" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="O5" s="1" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q5" s="1" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="S5" s="1" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U5" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="V5" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="X5" s="1" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="Y5" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="Z5" s="1" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="AA5" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:G1"/>
@@ -1558,7 +1744,7 @@
   <dimension ref="A1:E131"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="4:4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1568,77 +1754,77 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1648,19 +1834,19 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1668,13 +1854,13 @@
         <v>2</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1682,10 +1868,10 @@
         <v>3</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>31</v>
@@ -1696,10 +1882,10 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>32</v>
@@ -1710,13 +1896,13 @@
         <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1724,10 +1910,10 @@
         <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>32</v>
@@ -1738,10 +1924,10 @@
         <v>7</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1749,117 +1935,117 @@
         <v>8</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>32</v>
@@ -1870,161 +2056,161 @@
         <v>29</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2032,44 +2218,44 @@
         <v>9</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2077,214 +2263,214 @@
         <v>13</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2292,238 +2478,238 @@
         <v>29</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>32</v>
@@ -2531,16 +2717,16 @@
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2548,497 +2734,497 @@
         <v>29</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3046,55 +3232,55 @@
         <v>29</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="6" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="6" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -3120,7 +3306,7 @@
   <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="4:4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3130,77 +3316,77 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed recycling tests (#83)
</commit_message>
<xml_diff>
--- a/tests/data/20250616_ink_recycling_test.xlsx
+++ b/tests/data/20250616_ink_recycling_test.xlsx
@@ -8,9 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Experiment Data" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Data Entry Guide" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="How to Cite" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Experiment Data" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Data Entry Guide" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="How to Cite" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="297">
   <si>
     <t xml:space="preserve">Experiment Info</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t xml:space="preserve">MAI 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test recycling process 2</t>
   </si>
   <si>
     <t xml:space="preserve">Perovskite Solar Cell Fabrication Sequence</t>
@@ -922,7 +925,7 @@
   <fonts count="5">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -944,7 +947,7 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1122,190 +1125,15 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1f497d"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="eeece1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4f81bd"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="c0504d"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9bbb59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064a2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4bacc6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="f79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ff"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB8" activeCellId="0" sqref="AB8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q3" activeCellId="0" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1718,7 +1546,7 @@
         <v>85</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1737,7 +1565,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1754,77 +1582,77 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1834,19 +1662,19 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1854,13 +1682,13 @@
         <v>2</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1868,10 +1696,10 @@
         <v>3</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>31</v>
@@ -1882,10 +1710,10 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>32</v>
@@ -1896,10 +1724,10 @@
         <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>43</v>
@@ -1910,10 +1738,10 @@
         <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>32</v>
@@ -1924,10 +1752,10 @@
         <v>7</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1935,117 +1763,117 @@
         <v>8</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="E28" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>32</v>
@@ -2056,161 +1884,161 @@
         <v>29</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2218,44 +2046,44 @@
         <v>9</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2263,214 +2091,214 @@
         <v>13</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2478,238 +2306,238 @@
         <v>29</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E78" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D82" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>32</v>
@@ -2717,16 +2545,16 @@
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2734,497 +2562,497 @@
         <v>29</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E92" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3232,55 +3060,55 @@
         <v>29</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="6" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="6" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -3299,7 +3127,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3316,77 +3144,77 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>